<commit_message>
update du content matrix
</commit_message>
<xml_diff>
--- a/Documents/ContentMatrix_v2.1.xlsx
+++ b/Documents/ContentMatrix_v2.1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1322931\Desktop\SERVIDER\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1372883\Documents\Projet de bd\Servider\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="302">
   <si>
     <t>VERSION</t>
   </si>
@@ -918,6 +918,21 @@
   </si>
   <si>
     <t>Favorite Language</t>
+  </si>
+  <si>
+    <t>profil.btn.modifier</t>
+  </si>
+  <si>
+    <t>Bouton qui permet de modifier le profil</t>
+  </si>
+  <si>
+    <t>[Edit]</t>
+  </si>
+  <si>
+    <t>[Modifier]</t>
+  </si>
+  <si>
+    <t>11-12-2015</t>
   </si>
 </sst>
 </file>
@@ -1835,9 +1850,6 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1846,6 +1858,9 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="17" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="32">
@@ -2267,11 +2282,11 @@
   <sheetData>
     <row r="1" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="117" t="s">
+      <c r="B2" s="120" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="117"/>
-      <c r="D2" s="117"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="120"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" s="97" t="s">
@@ -2473,11 +2488,12 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:R855"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q63" sqref="Q63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2556,7 +2572,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" s="18" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="69"/>
       <c r="B2" s="55" t="s">
         <v>51</v>
@@ -2598,7 +2614,7 @@
       </c>
       <c r="R2" s="70"/>
     </row>
-    <row r="3" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" s="18" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="69"/>
       <c r="B3" s="55" t="s">
         <v>51</v>
@@ -2632,7 +2648,7 @@
       <c r="Q3" s="80"/>
       <c r="R3" s="70"/>
     </row>
-    <row r="4" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" s="18" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="36"/>
       <c r="B4" s="27" t="s">
         <v>51</v>
@@ -2676,7 +2692,7 @@
       </c>
       <c r="R4" s="34"/>
     </row>
-    <row r="5" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" s="18" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="36"/>
       <c r="B5" s="27" t="s">
         <v>51</v>
@@ -2720,7 +2736,7 @@
       </c>
       <c r="R5" s="34"/>
     </row>
-    <row r="6" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" s="18" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="36"/>
       <c r="B6" s="27" t="s">
         <v>51</v>
@@ -2764,7 +2780,7 @@
       </c>
       <c r="R6" s="34"/>
     </row>
-    <row r="7" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" s="18" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="36"/>
       <c r="B7" s="27" t="s">
         <v>51</v>
@@ -2808,7 +2824,7 @@
       </c>
       <c r="R7" s="34"/>
     </row>
-    <row r="8" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" s="18" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="36"/>
       <c r="B8" s="27" t="s">
         <v>51</v>
@@ -2852,7 +2868,7 @@
       </c>
       <c r="R8" s="34"/>
     </row>
-    <row r="9" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" s="18" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="36"/>
       <c r="B9" s="27" t="s">
         <v>67</v>
@@ -2894,7 +2910,7 @@
       </c>
       <c r="R9" s="34"/>
     </row>
-    <row r="10" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" s="18" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="36"/>
       <c r="B10" s="27" t="s">
         <v>67</v>
@@ -2936,7 +2952,7 @@
       </c>
       <c r="R10" s="34"/>
     </row>
-    <row r="11" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" s="18" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="36"/>
       <c r="B11" s="27" t="s">
         <v>67</v>
@@ -2978,7 +2994,7 @@
       </c>
       <c r="R11" s="34"/>
     </row>
-    <row r="12" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" s="18" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="36"/>
       <c r="B12" s="27" t="s">
         <v>67</v>
@@ -3020,7 +3036,7 @@
       </c>
       <c r="R12" s="34"/>
     </row>
-    <row r="13" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" s="18" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="36"/>
       <c r="B13" s="27" t="s">
         <v>67</v>
@@ -3062,7 +3078,7 @@
       </c>
       <c r="R13" s="34"/>
     </row>
-    <row r="14" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" s="18" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="36"/>
       <c r="B14" s="27" t="s">
         <v>67</v>
@@ -3104,7 +3120,7 @@
       </c>
       <c r="R14" s="34"/>
     </row>
-    <row r="15" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" s="18" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="36"/>
       <c r="B15" s="27" t="s">
         <v>67</v>
@@ -3146,7 +3162,7 @@
       </c>
       <c r="R15" s="34"/>
     </row>
-    <row r="16" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" s="18" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="36"/>
       <c r="B16" s="27" t="s">
         <v>67</v>
@@ -3188,7 +3204,7 @@
       </c>
       <c r="R16" s="34"/>
     </row>
-    <row r="17" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" s="18" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="36"/>
       <c r="B17" s="27" t="s">
         <v>67</v>
@@ -3230,7 +3246,7 @@
       </c>
       <c r="R17" s="34"/>
     </row>
-    <row r="18" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" s="18" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="36"/>
       <c r="B18" s="27" t="s">
         <v>67</v>
@@ -3272,7 +3288,7 @@
       </c>
       <c r="R18" s="34"/>
     </row>
-    <row r="19" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" s="18" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
       <c r="B19" s="27" t="s">
         <v>67</v>
@@ -3314,7 +3330,7 @@
       </c>
       <c r="R19" s="34"/>
     </row>
-    <row r="20" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" s="18" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="36"/>
       <c r="B20" s="27" t="s">
         <v>67</v>
@@ -3356,7 +3372,7 @@
       </c>
       <c r="R20" s="34"/>
     </row>
-    <row r="21" spans="1:18" s="18" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" s="18" customFormat="1" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="36"/>
       <c r="B21" s="27" t="s">
         <v>67</v>
@@ -3398,7 +3414,7 @@
       </c>
       <c r="R21" s="34"/>
     </row>
-    <row r="22" spans="1:18" s="18" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" s="18" customFormat="1" ht="50.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="36"/>
       <c r="B22" s="27" t="s">
         <v>67</v>
@@ -3440,7 +3456,7 @@
       </c>
       <c r="R22" s="34"/>
     </row>
-    <row r="23" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" s="18" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="36"/>
       <c r="B23" s="27" t="s">
         <v>67</v>
@@ -3482,7 +3498,7 @@
       </c>
       <c r="R23" s="34"/>
     </row>
-    <row r="24" spans="1:18" s="18" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" s="18" customFormat="1" ht="46.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="36"/>
       <c r="B24" s="27" t="s">
         <v>127</v>
@@ -3524,7 +3540,7 @@
       </c>
       <c r="R24" s="34"/>
     </row>
-    <row r="25" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" s="18" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="36"/>
       <c r="B25" s="27" t="s">
         <v>127</v>
@@ -3568,7 +3584,7 @@
       </c>
       <c r="R25" s="34"/>
     </row>
-    <row r="26" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18" s="18" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="36"/>
       <c r="B26" s="27" t="s">
         <v>127</v>
@@ -3610,7 +3626,7 @@
       </c>
       <c r="R26" s="34"/>
     </row>
-    <row r="27" spans="1:18" s="18" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" s="18" customFormat="1" ht="66.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="36"/>
       <c r="B27" s="27" t="s">
         <v>127</v>
@@ -3652,7 +3668,7 @@
       </c>
       <c r="R27" s="34"/>
     </row>
-    <row r="28" spans="1:18" s="18" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18" s="18" customFormat="1" ht="66.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="36"/>
       <c r="B28" s="27" t="s">
         <v>127</v>
@@ -3694,7 +3710,7 @@
       </c>
       <c r="R28" s="34"/>
     </row>
-    <row r="29" spans="1:18" s="18" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" s="18" customFormat="1" ht="42.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="69"/>
       <c r="B29" s="27" t="s">
         <v>127</v>
@@ -3736,7 +3752,7 @@
       </c>
       <c r="R29" s="70"/>
     </row>
-    <row r="30" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18" s="18" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="36"/>
       <c r="B30" s="27" t="s">
         <v>127</v>
@@ -3778,7 +3794,7 @@
       </c>
       <c r="R30" s="34"/>
     </row>
-    <row r="31" spans="1:18" s="18" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18" s="18" customFormat="1" ht="57" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="36"/>
       <c r="B31" s="27" t="s">
         <v>150</v>
@@ -3820,7 +3836,7 @@
       </c>
       <c r="R31" s="34"/>
     </row>
-    <row r="32" spans="1:18" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18" s="18" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="36"/>
       <c r="B32" s="27" t="s">
         <v>150</v>
@@ -3988,7 +4004,7 @@
       </c>
       <c r="R35" s="34"/>
     </row>
-    <row r="36" spans="1:18" s="18" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A36" s="36"/>
       <c r="B36" s="27" t="s">
         <v>161</v>
@@ -4030,7 +4046,7 @@
       </c>
       <c r="R36" s="34"/>
     </row>
-    <row r="37" spans="1:18" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" s="18" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B37" s="27" t="s">
         <v>178</v>
       </c>
@@ -4071,7 +4087,7 @@
       </c>
       <c r="R37" s="34"/>
     </row>
-    <row r="38" spans="1:18" s="18" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:18" s="18" customFormat="1" ht="35.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="36"/>
       <c r="B38" s="27" t="s">
         <v>178</v>
@@ -4113,7 +4129,7 @@
       </c>
       <c r="R38" s="34"/>
     </row>
-    <row r="39" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:18" s="18" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="36"/>
       <c r="B39" s="27" t="s">
         <v>178</v>
@@ -4155,7 +4171,7 @@
       </c>
       <c r="R39" s="34"/>
     </row>
-    <row r="40" spans="1:18" s="81" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:18" s="81" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="36"/>
       <c r="B40" s="27" t="s">
         <v>178</v>
@@ -4197,7 +4213,7 @@
       </c>
       <c r="R40" s="34"/>
     </row>
-    <row r="41" spans="1:18" s="81" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:18" s="81" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="36"/>
       <c r="B41" s="27" t="s">
         <v>178</v>
@@ -4239,7 +4255,7 @@
       </c>
       <c r="R41" s="34"/>
     </row>
-    <row r="42" spans="1:18" s="81" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:18" s="81" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="69"/>
       <c r="B42" s="55" t="s">
         <v>178</v>
@@ -4281,7 +4297,7 @@
       </c>
       <c r="R42" s="70"/>
     </row>
-    <row r="43" spans="1:18" s="81" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:18" s="81" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="36"/>
       <c r="B43" s="27" t="s">
         <v>178</v>
@@ -4323,7 +4339,7 @@
       </c>
       <c r="R43" s="34"/>
     </row>
-    <row r="44" spans="1:18" s="81" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:18" s="81" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="36"/>
       <c r="B44" s="27" t="s">
         <v>263</v>
@@ -4367,7 +4383,7 @@
       </c>
       <c r="R44" s="34"/>
     </row>
-    <row r="45" spans="1:18" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:18" s="18" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="36"/>
       <c r="B45" s="27" t="s">
         <v>263</v>
@@ -4411,7 +4427,7 @@
       </c>
       <c r="R45" s="34"/>
     </row>
-    <row r="46" spans="1:18" s="21" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:18" s="21" customFormat="1" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="36"/>
       <c r="B46" s="27" t="s">
         <v>263</v>
@@ -4455,7 +4471,7 @@
       </c>
       <c r="R46" s="34"/>
     </row>
-    <row r="47" spans="1:18" s="21" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:18" s="21" customFormat="1" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="36"/>
       <c r="B47" s="27" t="s">
         <v>264</v>
@@ -4499,7 +4515,7 @@
       </c>
       <c r="R47" s="34"/>
     </row>
-    <row r="48" spans="1:18" s="21" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:18" s="21" customFormat="1" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="36"/>
       <c r="B48" s="27" t="s">
         <v>264</v>
@@ -4543,7 +4559,7 @@
       </c>
       <c r="R48" s="34"/>
     </row>
-    <row r="49" spans="1:18" s="21" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:18" s="21" customFormat="1" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="36"/>
       <c r="B49" s="27" t="s">
         <v>264</v>
@@ -4587,7 +4603,7 @@
       </c>
       <c r="R49" s="34"/>
     </row>
-    <row r="50" spans="1:18" s="21" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:18" s="21" customFormat="1" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="36"/>
       <c r="B50" s="27" t="s">
         <v>264</v>
@@ -4631,7 +4647,7 @@
       </c>
       <c r="R50" s="34"/>
     </row>
-    <row r="51" spans="1:18" s="21" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" s="21" customFormat="1" ht="27" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A51" s="36"/>
       <c r="B51" s="27" t="s">
         <v>264</v>
@@ -4675,7 +4691,7 @@
       </c>
       <c r="R51" s="34"/>
     </row>
-    <row r="52" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" s="18" customFormat="1" ht="28.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="36"/>
       <c r="B52" s="27" t="s">
         <v>227</v>
@@ -4717,7 +4733,7 @@
       </c>
       <c r="R52" s="34"/>
     </row>
-    <row r="53" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" s="18" customFormat="1" ht="28.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="36"/>
       <c r="B53" s="27" t="s">
         <v>227</v>
@@ -4759,7 +4775,7 @@
       </c>
       <c r="R53" s="34"/>
     </row>
-    <row r="54" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" s="18" customFormat="1" ht="28.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="36"/>
       <c r="B54" s="27" t="s">
         <v>227</v>
@@ -4801,7 +4817,7 @@
       </c>
       <c r="R54" s="34"/>
     </row>
-    <row r="55" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" s="18" customFormat="1" ht="28.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="36"/>
       <c r="B55" s="27" t="s">
         <v>227</v>
@@ -4843,7 +4859,7 @@
       </c>
       <c r="R55" s="34"/>
     </row>
-    <row r="56" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" s="18" customFormat="1" ht="28.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A56" s="36"/>
       <c r="B56" s="27" t="s">
         <v>227</v>
@@ -4885,7 +4901,7 @@
       </c>
       <c r="R56" s="34"/>
     </row>
-    <row r="57" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" s="18" customFormat="1" ht="28.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="36"/>
       <c r="B57" s="27" t="s">
         <v>227</v>
@@ -4927,7 +4943,7 @@
       </c>
       <c r="R57" s="34"/>
     </row>
-    <row r="58" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" s="18" customFormat="1" ht="28.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="36"/>
       <c r="B58" s="27" t="s">
         <v>227</v>
@@ -4969,7 +4985,7 @@
       </c>
       <c r="R58" s="34"/>
     </row>
-    <row r="59" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" s="18" customFormat="1" ht="28.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="36"/>
       <c r="B59" s="27" t="s">
         <v>227</v>
@@ -5011,7 +5027,7 @@
       </c>
       <c r="R59" s="34"/>
     </row>
-    <row r="60" spans="1:18" s="18" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:18" s="18" customFormat="1" ht="42" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="36"/>
       <c r="B60" s="27" t="s">
         <v>67</v>
@@ -5053,7 +5069,7 @@
       </c>
       <c r="R60" s="34"/>
     </row>
-    <row r="61" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:18" s="18" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="36"/>
       <c r="B61" s="27" t="s">
         <v>67</v>
@@ -5097,22 +5113,44 @@
     </row>
     <row r="62" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="36"/>
-      <c r="B62" s="27"/>
-      <c r="C62" s="43"/>
+      <c r="B62" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="C62" s="43">
+        <v>5</v>
+      </c>
       <c r="D62" s="34"/>
-      <c r="E62" s="39"/>
-      <c r="F62" s="37"/>
-      <c r="G62" s="27"/>
-      <c r="H62" s="27"/>
-      <c r="I62" s="27"/>
-      <c r="J62" s="54"/>
-      <c r="K62" s="118"/>
+      <c r="E62" s="39" t="s">
+        <v>297</v>
+      </c>
+      <c r="F62" s="37" t="s">
+        <v>174</v>
+      </c>
+      <c r="G62" s="27" t="s">
+        <v>298</v>
+      </c>
+      <c r="H62" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="I62" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="J62" s="40" t="s">
+        <v>299</v>
+      </c>
+      <c r="K62" s="40" t="s">
+        <v>300</v>
+      </c>
       <c r="L62" s="28"/>
       <c r="M62" s="28"/>
       <c r="N62" s="28"/>
       <c r="O62" s="28"/>
-      <c r="P62" s="25"/>
-      <c r="Q62" s="26"/>
+      <c r="P62" s="25" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q62" s="26" t="s">
+        <v>301</v>
+      </c>
       <c r="R62" s="34"/>
     </row>
     <row r="63" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -5126,7 +5164,7 @@
       <c r="H63" s="27"/>
       <c r="I63" s="27"/>
       <c r="J63" s="54"/>
-      <c r="K63" s="118"/>
+      <c r="K63" s="117"/>
       <c r="L63" s="28"/>
       <c r="M63" s="28"/>
       <c r="N63" s="28"/>
@@ -5306,7 +5344,7 @@
       <c r="H72" s="27"/>
       <c r="I72" s="27"/>
       <c r="J72" s="54"/>
-      <c r="K72" s="118"/>
+      <c r="K72" s="117"/>
       <c r="L72" s="28"/>
       <c r="M72" s="28"/>
       <c r="N72" s="28"/>
@@ -5326,7 +5364,7 @@
       <c r="H73" s="27"/>
       <c r="I73" s="27"/>
       <c r="J73" s="54"/>
-      <c r="K73" s="118"/>
+      <c r="K73" s="117"/>
       <c r="L73" s="28"/>
       <c r="M73" s="28"/>
       <c r="N73" s="28"/>
@@ -5366,7 +5404,7 @@
       <c r="H75" s="27"/>
       <c r="I75" s="27"/>
       <c r="J75" s="54"/>
-      <c r="K75" s="118"/>
+      <c r="K75" s="117"/>
       <c r="L75" s="28"/>
       <c r="M75" s="28"/>
       <c r="N75" s="28"/>
@@ -5386,7 +5424,7 @@
       <c r="H76" s="27"/>
       <c r="I76" s="27"/>
       <c r="J76" s="54"/>
-      <c r="K76" s="118"/>
+      <c r="K76" s="117"/>
       <c r="L76" s="28"/>
       <c r="M76" s="28"/>
       <c r="N76" s="28"/>
@@ -5426,7 +5464,7 @@
       <c r="H78" s="27"/>
       <c r="I78" s="27"/>
       <c r="J78" s="54"/>
-      <c r="K78" s="118"/>
+      <c r="K78" s="117"/>
       <c r="L78" s="28"/>
       <c r="M78" s="28"/>
       <c r="N78" s="28"/>
@@ -5546,7 +5584,7 @@
       <c r="H84" s="27"/>
       <c r="I84" s="27"/>
       <c r="J84" s="54"/>
-      <c r="K84" s="118"/>
+      <c r="K84" s="117"/>
       <c r="L84" s="28"/>
       <c r="M84" s="28"/>
       <c r="N84" s="28"/>
@@ -5626,7 +5664,7 @@
       <c r="H88" s="27"/>
       <c r="I88" s="27"/>
       <c r="J88" s="54"/>
-      <c r="K88" s="118"/>
+      <c r="K88" s="117"/>
       <c r="L88" s="28"/>
       <c r="M88" s="28"/>
       <c r="N88" s="28"/>
@@ -5686,7 +5724,7 @@
       <c r="H91" s="27"/>
       <c r="I91" s="27"/>
       <c r="J91" s="54"/>
-      <c r="K91" s="118"/>
+      <c r="K91" s="117"/>
       <c r="L91" s="28"/>
       <c r="M91" s="28"/>
       <c r="N91" s="28"/>
@@ -6026,7 +6064,7 @@
       <c r="H108" s="27"/>
       <c r="I108" s="27"/>
       <c r="J108" s="54"/>
-      <c r="K108" s="118"/>
+      <c r="K108" s="117"/>
       <c r="L108" s="28"/>
       <c r="M108" s="28"/>
       <c r="N108" s="28"/>
@@ -6046,7 +6084,7 @@
       <c r="H109" s="27"/>
       <c r="I109" s="27"/>
       <c r="J109" s="54"/>
-      <c r="K109" s="118"/>
+      <c r="K109" s="117"/>
       <c r="L109" s="28"/>
       <c r="M109" s="28"/>
       <c r="N109" s="28"/>
@@ -6206,7 +6244,7 @@
       <c r="H117" s="38"/>
       <c r="I117" s="38"/>
       <c r="J117" s="54"/>
-      <c r="K117" s="118"/>
+      <c r="K117" s="117"/>
       <c r="L117" s="30"/>
       <c r="M117" s="30"/>
       <c r="N117" s="30"/>
@@ -6226,7 +6264,7 @@
       <c r="H118" s="38"/>
       <c r="I118" s="38"/>
       <c r="J118" s="54"/>
-      <c r="K118" s="118"/>
+      <c r="K118" s="117"/>
       <c r="L118" s="30"/>
       <c r="M118" s="30"/>
       <c r="N118" s="30"/>
@@ -6426,7 +6464,7 @@
       <c r="H128" s="27"/>
       <c r="I128" s="27"/>
       <c r="J128" s="54"/>
-      <c r="K128" s="118"/>
+      <c r="K128" s="117"/>
       <c r="L128" s="28"/>
       <c r="M128" s="28"/>
       <c r="N128" s="28"/>
@@ -6446,7 +6484,7 @@
       <c r="H129" s="27"/>
       <c r="I129" s="27"/>
       <c r="J129" s="54"/>
-      <c r="K129" s="118"/>
+      <c r="K129" s="117"/>
       <c r="L129" s="28"/>
       <c r="M129" s="28"/>
       <c r="N129" s="28"/>
@@ -6466,7 +6504,7 @@
       <c r="H130" s="27"/>
       <c r="I130" s="27"/>
       <c r="J130" s="54"/>
-      <c r="K130" s="118"/>
+      <c r="K130" s="117"/>
       <c r="L130" s="28"/>
       <c r="M130" s="28"/>
       <c r="N130" s="28"/>
@@ -6526,7 +6564,7 @@
       <c r="H133" s="38"/>
       <c r="I133" s="38"/>
       <c r="J133" s="54"/>
-      <c r="K133" s="118"/>
+      <c r="K133" s="117"/>
       <c r="L133" s="30"/>
       <c r="M133" s="30"/>
       <c r="N133" s="30"/>
@@ -6646,7 +6684,7 @@
       <c r="H139" s="27"/>
       <c r="I139" s="27"/>
       <c r="J139" s="54"/>
-      <c r="K139" s="118"/>
+      <c r="K139" s="117"/>
       <c r="L139" s="28"/>
       <c r="M139" s="28"/>
       <c r="N139" s="28"/>
@@ -6666,7 +6704,7 @@
       <c r="H140" s="27"/>
       <c r="I140" s="27"/>
       <c r="J140" s="54"/>
-      <c r="K140" s="118"/>
+      <c r="K140" s="117"/>
       <c r="L140" s="28"/>
       <c r="M140" s="28"/>
       <c r="N140" s="28"/>
@@ -6686,7 +6724,7 @@
       <c r="H141" s="27"/>
       <c r="I141" s="27"/>
       <c r="J141" s="54"/>
-      <c r="K141" s="118"/>
+      <c r="K141" s="117"/>
       <c r="L141" s="28"/>
       <c r="M141" s="28"/>
       <c r="N141" s="28"/>
@@ -6706,7 +6744,7 @@
       <c r="H142" s="27"/>
       <c r="I142" s="27"/>
       <c r="J142" s="54"/>
-      <c r="K142" s="118"/>
+      <c r="K142" s="117"/>
       <c r="L142" s="28"/>
       <c r="M142" s="28"/>
       <c r="N142" s="28"/>
@@ -6726,7 +6764,7 @@
       <c r="H143" s="27"/>
       <c r="I143" s="27"/>
       <c r="J143" s="54"/>
-      <c r="K143" s="118"/>
+      <c r="K143" s="117"/>
       <c r="L143" s="28"/>
       <c r="M143" s="28"/>
       <c r="N143" s="28"/>
@@ -6766,7 +6804,7 @@
       <c r="H145" s="27"/>
       <c r="I145" s="27"/>
       <c r="J145" s="54"/>
-      <c r="K145" s="118"/>
+      <c r="K145" s="117"/>
       <c r="L145" s="28"/>
       <c r="M145" s="28"/>
       <c r="N145" s="28"/>
@@ -6786,7 +6824,7 @@
       <c r="H146" s="27"/>
       <c r="I146" s="27"/>
       <c r="J146" s="54"/>
-      <c r="K146" s="118"/>
+      <c r="K146" s="117"/>
       <c r="L146" s="28"/>
       <c r="M146" s="28"/>
       <c r="N146" s="28"/>
@@ -7026,7 +7064,7 @@
       <c r="H158" s="38"/>
       <c r="I158" s="38"/>
       <c r="J158" s="54"/>
-      <c r="K158" s="118"/>
+      <c r="K158" s="117"/>
       <c r="L158" s="30"/>
       <c r="M158" s="30"/>
       <c r="N158" s="30"/>
@@ -7046,7 +7084,7 @@
       <c r="H159" s="38"/>
       <c r="I159" s="38"/>
       <c r="J159" s="54"/>
-      <c r="K159" s="118"/>
+      <c r="K159" s="117"/>
       <c r="L159" s="30"/>
       <c r="M159" s="30"/>
       <c r="N159" s="30"/>
@@ -7066,7 +7104,7 @@
       <c r="H160" s="38"/>
       <c r="I160" s="38"/>
       <c r="J160" s="54"/>
-      <c r="K160" s="118"/>
+      <c r="K160" s="117"/>
       <c r="L160" s="30"/>
       <c r="M160" s="30"/>
       <c r="N160" s="30"/>
@@ -7106,7 +7144,7 @@
       <c r="H162" s="62"/>
       <c r="I162" s="62"/>
       <c r="J162" s="88"/>
-      <c r="K162" s="119"/>
+      <c r="K162" s="118"/>
       <c r="L162" s="66"/>
       <c r="M162" s="66"/>
       <c r="N162" s="66"/>
@@ -7126,7 +7164,7 @@
       <c r="H163" s="38"/>
       <c r="I163" s="38"/>
       <c r="J163" s="54"/>
-      <c r="K163" s="118"/>
+      <c r="K163" s="117"/>
       <c r="L163" s="30"/>
       <c r="M163" s="30"/>
       <c r="N163" s="30"/>
@@ -7486,7 +7524,7 @@
       <c r="H181" s="38"/>
       <c r="I181" s="38"/>
       <c r="J181" s="54"/>
-      <c r="K181" s="118"/>
+      <c r="K181" s="117"/>
       <c r="L181" s="30"/>
       <c r="M181" s="30"/>
       <c r="N181" s="30"/>
@@ -7726,7 +7764,7 @@
       <c r="H193" s="27"/>
       <c r="I193" s="27"/>
       <c r="J193" s="54"/>
-      <c r="K193" s="118"/>
+      <c r="K193" s="117"/>
       <c r="L193" s="28"/>
       <c r="M193" s="28"/>
       <c r="N193" s="28"/>
@@ -7746,7 +7784,7 @@
       <c r="H194" s="27"/>
       <c r="I194" s="27"/>
       <c r="J194" s="54"/>
-      <c r="K194" s="118"/>
+      <c r="K194" s="117"/>
       <c r="L194" s="28"/>
       <c r="M194" s="28"/>
       <c r="N194" s="28"/>
@@ -7766,7 +7804,7 @@
       <c r="H195" s="27"/>
       <c r="I195" s="27"/>
       <c r="J195" s="54"/>
-      <c r="K195" s="118"/>
+      <c r="K195" s="117"/>
       <c r="L195" s="28"/>
       <c r="M195" s="28"/>
       <c r="N195" s="28"/>
@@ -7786,7 +7824,7 @@
       <c r="H196" s="27"/>
       <c r="I196" s="27"/>
       <c r="J196" s="54"/>
-      <c r="K196" s="118"/>
+      <c r="K196" s="117"/>
       <c r="L196" s="28"/>
       <c r="M196" s="28"/>
       <c r="N196" s="28"/>
@@ -7806,7 +7844,7 @@
       <c r="H197" s="27"/>
       <c r="I197" s="27"/>
       <c r="J197" s="54"/>
-      <c r="K197" s="118"/>
+      <c r="K197" s="117"/>
       <c r="L197" s="28"/>
       <c r="M197" s="28"/>
       <c r="N197" s="28"/>
@@ -7886,7 +7924,7 @@
       <c r="H201" s="27"/>
       <c r="I201" s="27"/>
       <c r="J201" s="54"/>
-      <c r="K201" s="118"/>
+      <c r="K201" s="117"/>
       <c r="L201" s="28"/>
       <c r="M201" s="28"/>
       <c r="N201" s="28"/>
@@ -7906,7 +7944,7 @@
       <c r="H202" s="27"/>
       <c r="I202" s="27"/>
       <c r="J202" s="54"/>
-      <c r="K202" s="118"/>
+      <c r="K202" s="117"/>
       <c r="L202" s="28"/>
       <c r="M202" s="28"/>
       <c r="N202" s="28"/>
@@ -7926,7 +7964,7 @@
       <c r="H203" s="27"/>
       <c r="I203" s="27"/>
       <c r="J203" s="54"/>
-      <c r="K203" s="118"/>
+      <c r="K203" s="117"/>
       <c r="L203" s="28"/>
       <c r="M203" s="28"/>
       <c r="N203" s="28"/>
@@ -7946,7 +7984,7 @@
       <c r="H204" s="27"/>
       <c r="I204" s="27"/>
       <c r="J204" s="54"/>
-      <c r="K204" s="118"/>
+      <c r="K204" s="117"/>
       <c r="L204" s="28"/>
       <c r="M204" s="28"/>
       <c r="N204" s="28"/>
@@ -7966,7 +8004,7 @@
       <c r="H205" s="27"/>
       <c r="I205" s="27"/>
       <c r="J205" s="54"/>
-      <c r="K205" s="118"/>
+      <c r="K205" s="117"/>
       <c r="L205" s="28"/>
       <c r="M205" s="28"/>
       <c r="N205" s="28"/>
@@ -8066,7 +8104,7 @@
       <c r="H210" s="38"/>
       <c r="I210" s="38"/>
       <c r="J210" s="54"/>
-      <c r="K210" s="118"/>
+      <c r="K210" s="117"/>
       <c r="L210" s="30"/>
       <c r="M210" s="30"/>
       <c r="N210" s="30"/>
@@ -8086,7 +8124,7 @@
       <c r="H211" s="38"/>
       <c r="I211" s="38"/>
       <c r="J211" s="54"/>
-      <c r="K211" s="118"/>
+      <c r="K211" s="117"/>
       <c r="L211" s="30"/>
       <c r="M211" s="30"/>
       <c r="N211" s="30"/>
@@ -8106,7 +8144,7 @@
       <c r="H212" s="38"/>
       <c r="I212" s="38"/>
       <c r="J212" s="54"/>
-      <c r="K212" s="118"/>
+      <c r="K212" s="117"/>
       <c r="L212" s="30"/>
       <c r="M212" s="30"/>
       <c r="N212" s="30"/>
@@ -8126,7 +8164,7 @@
       <c r="H213" s="38"/>
       <c r="I213" s="38"/>
       <c r="J213" s="54"/>
-      <c r="K213" s="118"/>
+      <c r="K213" s="117"/>
       <c r="L213" s="30"/>
       <c r="M213" s="30"/>
       <c r="N213" s="30"/>
@@ -8146,7 +8184,7 @@
       <c r="H214" s="38"/>
       <c r="I214" s="38"/>
       <c r="J214" s="54"/>
-      <c r="K214" s="118"/>
+      <c r="K214" s="117"/>
       <c r="L214" s="30"/>
       <c r="M214" s="30"/>
       <c r="N214" s="30"/>
@@ -8166,7 +8204,7 @@
       <c r="H215" s="38"/>
       <c r="I215" s="38"/>
       <c r="J215" s="54"/>
-      <c r="K215" s="118"/>
+      <c r="K215" s="117"/>
       <c r="L215" s="30"/>
       <c r="M215" s="30"/>
       <c r="N215" s="30"/>
@@ -8186,7 +8224,7 @@
       <c r="H216" s="38"/>
       <c r="I216" s="38"/>
       <c r="J216" s="54"/>
-      <c r="K216" s="118"/>
+      <c r="K216" s="117"/>
       <c r="L216" s="30"/>
       <c r="M216" s="30"/>
       <c r="N216" s="30"/>
@@ -8226,7 +8264,7 @@
       <c r="H218" s="38"/>
       <c r="I218" s="38"/>
       <c r="J218" s="54"/>
-      <c r="K218" s="118"/>
+      <c r="K218" s="117"/>
       <c r="L218" s="30"/>
       <c r="M218" s="30"/>
       <c r="N218" s="30"/>
@@ -8246,7 +8284,7 @@
       <c r="H219" s="38"/>
       <c r="I219" s="38"/>
       <c r="J219" s="54"/>
-      <c r="K219" s="118"/>
+      <c r="K219" s="117"/>
       <c r="L219" s="30"/>
       <c r="M219" s="30"/>
       <c r="N219" s="30"/>
@@ -8606,7 +8644,7 @@
       <c r="H237" s="27"/>
       <c r="I237" s="27"/>
       <c r="J237" s="54"/>
-      <c r="K237" s="118"/>
+      <c r="K237" s="117"/>
       <c r="L237" s="28"/>
       <c r="M237" s="28"/>
       <c r="N237" s="28"/>
@@ -8626,7 +8664,7 @@
       <c r="H238" s="27"/>
       <c r="I238" s="27"/>
       <c r="J238" s="54"/>
-      <c r="K238" s="118"/>
+      <c r="K238" s="117"/>
       <c r="L238" s="28"/>
       <c r="M238" s="28"/>
       <c r="N238" s="28"/>
@@ -8746,7 +8784,7 @@
       <c r="H244" s="38"/>
       <c r="I244" s="38"/>
       <c r="J244" s="54"/>
-      <c r="K244" s="118"/>
+      <c r="K244" s="117"/>
       <c r="L244" s="30"/>
       <c r="M244" s="30"/>
       <c r="N244" s="30"/>
@@ -9546,7 +9584,7 @@
       <c r="H284" s="27"/>
       <c r="I284" s="27"/>
       <c r="J284" s="54"/>
-      <c r="K284" s="118"/>
+      <c r="K284" s="117"/>
       <c r="L284" s="28"/>
       <c r="M284" s="28"/>
       <c r="N284" s="28"/>
@@ -9586,7 +9624,7 @@
       <c r="H286" s="27"/>
       <c r="I286" s="27"/>
       <c r="J286" s="54"/>
-      <c r="K286" s="118"/>
+      <c r="K286" s="117"/>
       <c r="L286" s="28"/>
       <c r="M286" s="28"/>
       <c r="N286" s="28"/>
@@ -9706,7 +9744,7 @@
       <c r="H292" s="38"/>
       <c r="I292" s="38"/>
       <c r="J292" s="54"/>
-      <c r="K292" s="118"/>
+      <c r="K292" s="117"/>
       <c r="L292" s="30"/>
       <c r="M292" s="30"/>
       <c r="N292" s="30"/>
@@ -9726,7 +9764,7 @@
       <c r="H293" s="38"/>
       <c r="I293" s="38"/>
       <c r="J293" s="54"/>
-      <c r="K293" s="118"/>
+      <c r="K293" s="117"/>
       <c r="L293" s="30"/>
       <c r="M293" s="30"/>
       <c r="N293" s="30"/>
@@ -11766,7 +11804,7 @@
       <c r="H395" s="38"/>
       <c r="I395" s="38"/>
       <c r="J395" s="54"/>
-      <c r="K395" s="118"/>
+      <c r="K395" s="117"/>
       <c r="L395" s="30"/>
       <c r="M395" s="30"/>
       <c r="N395" s="30"/>
@@ -11786,7 +11824,7 @@
       <c r="H396" s="38"/>
       <c r="I396" s="38"/>
       <c r="J396" s="54"/>
-      <c r="K396" s="118"/>
+      <c r="K396" s="117"/>
       <c r="L396" s="30"/>
       <c r="M396" s="30"/>
       <c r="N396" s="30"/>
@@ -11806,7 +11844,7 @@
       <c r="H397" s="38"/>
       <c r="I397" s="38"/>
       <c r="J397" s="54"/>
-      <c r="K397" s="118"/>
+      <c r="K397" s="117"/>
       <c r="L397" s="30"/>
       <c r="M397" s="30"/>
       <c r="N397" s="30"/>
@@ -11826,7 +11864,7 @@
       <c r="H398" s="38"/>
       <c r="I398" s="38"/>
       <c r="J398" s="54"/>
-      <c r="K398" s="118"/>
+      <c r="K398" s="117"/>
       <c r="L398" s="30"/>
       <c r="M398" s="30"/>
       <c r="N398" s="30"/>
@@ -12306,7 +12344,7 @@
       <c r="H422" s="38"/>
       <c r="I422" s="38"/>
       <c r="J422" s="54"/>
-      <c r="K422" s="118"/>
+      <c r="K422" s="117"/>
       <c r="L422" s="30"/>
       <c r="M422" s="30"/>
       <c r="N422" s="30"/>
@@ -12326,7 +12364,7 @@
       <c r="H423" s="38"/>
       <c r="I423" s="38"/>
       <c r="J423" s="54"/>
-      <c r="K423" s="118"/>
+      <c r="K423" s="117"/>
       <c r="L423" s="30"/>
       <c r="M423" s="30"/>
       <c r="N423" s="30"/>
@@ -12346,7 +12384,7 @@
       <c r="H424" s="38"/>
       <c r="I424" s="38"/>
       <c r="J424" s="54"/>
-      <c r="K424" s="118"/>
+      <c r="K424" s="117"/>
       <c r="L424" s="30"/>
       <c r="M424" s="30"/>
       <c r="N424" s="30"/>
@@ -12366,7 +12404,7 @@
       <c r="H425" s="38"/>
       <c r="I425" s="38"/>
       <c r="J425" s="54"/>
-      <c r="K425" s="118"/>
+      <c r="K425" s="117"/>
       <c r="L425" s="30"/>
       <c r="M425" s="30"/>
       <c r="N425" s="30"/>
@@ -12386,7 +12424,7 @@
       <c r="H426" s="38"/>
       <c r="I426" s="38"/>
       <c r="J426" s="54"/>
-      <c r="K426" s="118"/>
+      <c r="K426" s="117"/>
       <c r="L426" s="30"/>
       <c r="M426" s="30"/>
       <c r="N426" s="30"/>
@@ -12406,7 +12444,7 @@
       <c r="H427" s="38"/>
       <c r="I427" s="38"/>
       <c r="J427" s="54"/>
-      <c r="K427" s="118"/>
+      <c r="K427" s="117"/>
       <c r="L427" s="30"/>
       <c r="M427" s="30"/>
       <c r="N427" s="30"/>
@@ -12426,7 +12464,7 @@
       <c r="H428" s="38"/>
       <c r="I428" s="38"/>
       <c r="J428" s="54"/>
-      <c r="K428" s="118"/>
+      <c r="K428" s="117"/>
       <c r="L428" s="30"/>
       <c r="M428" s="30"/>
       <c r="N428" s="30"/>
@@ -12446,7 +12484,7 @@
       <c r="H429" s="38"/>
       <c r="I429" s="38"/>
       <c r="J429" s="54"/>
-      <c r="K429" s="118"/>
+      <c r="K429" s="117"/>
       <c r="L429" s="30"/>
       <c r="M429" s="30"/>
       <c r="N429" s="30"/>
@@ -12466,7 +12504,7 @@
       <c r="H430" s="38"/>
       <c r="I430" s="38"/>
       <c r="J430" s="54"/>
-      <c r="K430" s="118"/>
+      <c r="K430" s="117"/>
       <c r="L430" s="30"/>
       <c r="M430" s="30"/>
       <c r="N430" s="30"/>
@@ -12486,7 +12524,7 @@
       <c r="H431" s="38"/>
       <c r="I431" s="38"/>
       <c r="J431" s="54"/>
-      <c r="K431" s="118"/>
+      <c r="K431" s="117"/>
       <c r="L431" s="30"/>
       <c r="M431" s="30"/>
       <c r="N431" s="30"/>
@@ -12506,7 +12544,7 @@
       <c r="H432" s="38"/>
       <c r="I432" s="38"/>
       <c r="J432" s="54"/>
-      <c r="K432" s="118"/>
+      <c r="K432" s="117"/>
       <c r="L432" s="30"/>
       <c r="M432" s="30"/>
       <c r="N432" s="30"/>
@@ -12606,7 +12644,7 @@
       <c r="H437" s="38"/>
       <c r="I437" s="38"/>
       <c r="J437" s="54"/>
-      <c r="K437" s="118"/>
+      <c r="K437" s="117"/>
       <c r="L437" s="30"/>
       <c r="M437" s="30"/>
       <c r="N437" s="30"/>
@@ -12626,7 +12664,7 @@
       <c r="H438" s="38"/>
       <c r="I438" s="38"/>
       <c r="J438" s="54"/>
-      <c r="K438" s="118"/>
+      <c r="K438" s="117"/>
       <c r="L438" s="30"/>
       <c r="M438" s="30"/>
       <c r="N438" s="30"/>
@@ -12646,7 +12684,7 @@
       <c r="H439" s="38"/>
       <c r="I439" s="38"/>
       <c r="J439" s="54"/>
-      <c r="K439" s="118"/>
+      <c r="K439" s="117"/>
       <c r="L439" s="30"/>
       <c r="M439" s="30"/>
       <c r="N439" s="30"/>
@@ -13086,7 +13124,7 @@
       <c r="H461" s="38"/>
       <c r="I461" s="38"/>
       <c r="J461" s="54"/>
-      <c r="K461" s="118"/>
+      <c r="K461" s="117"/>
       <c r="L461" s="30"/>
       <c r="M461" s="30"/>
       <c r="N461" s="30"/>
@@ -13366,7 +13404,7 @@
       <c r="H475" s="38"/>
       <c r="I475" s="38"/>
       <c r="J475" s="54"/>
-      <c r="K475" s="118"/>
+      <c r="K475" s="117"/>
       <c r="L475" s="30"/>
       <c r="M475" s="30"/>
       <c r="N475" s="30"/>
@@ -14306,7 +14344,7 @@
       <c r="H522" s="38"/>
       <c r="I522" s="38"/>
       <c r="J522" s="54"/>
-      <c r="K522" s="118"/>
+      <c r="K522" s="117"/>
       <c r="L522" s="30"/>
       <c r="M522" s="30"/>
       <c r="N522" s="30"/>
@@ -14326,7 +14364,7 @@
       <c r="H523" s="38"/>
       <c r="I523" s="38"/>
       <c r="J523" s="54"/>
-      <c r="K523" s="118"/>
+      <c r="K523" s="117"/>
       <c r="L523" s="30"/>
       <c r="M523" s="30"/>
       <c r="N523" s="30"/>
@@ -14346,7 +14384,7 @@
       <c r="H524" s="38"/>
       <c r="I524" s="38"/>
       <c r="J524" s="54"/>
-      <c r="K524" s="118"/>
+      <c r="K524" s="117"/>
       <c r="L524" s="30"/>
       <c r="M524" s="30"/>
       <c r="N524" s="30"/>
@@ -14366,7 +14404,7 @@
       <c r="H525" s="38"/>
       <c r="I525" s="38"/>
       <c r="J525" s="54"/>
-      <c r="K525" s="118"/>
+      <c r="K525" s="117"/>
       <c r="L525" s="30"/>
       <c r="M525" s="30"/>
       <c r="N525" s="30"/>
@@ -14386,7 +14424,7 @@
       <c r="H526" s="38"/>
       <c r="I526" s="38"/>
       <c r="J526" s="54"/>
-      <c r="K526" s="118"/>
+      <c r="K526" s="117"/>
       <c r="L526" s="30"/>
       <c r="M526" s="30"/>
       <c r="N526" s="30"/>
@@ -14406,7 +14444,7 @@
       <c r="H527" s="38"/>
       <c r="I527" s="38"/>
       <c r="J527" s="54"/>
-      <c r="K527" s="118"/>
+      <c r="K527" s="117"/>
       <c r="L527" s="30"/>
       <c r="M527" s="30"/>
       <c r="N527" s="30"/>
@@ -14426,7 +14464,7 @@
       <c r="H528" s="38"/>
       <c r="I528" s="38"/>
       <c r="J528" s="54"/>
-      <c r="K528" s="118"/>
+      <c r="K528" s="117"/>
       <c r="L528" s="30"/>
       <c r="M528" s="30"/>
       <c r="N528" s="30"/>
@@ -14446,7 +14484,7 @@
       <c r="H529" s="38"/>
       <c r="I529" s="38"/>
       <c r="J529" s="54"/>
-      <c r="K529" s="118"/>
+      <c r="K529" s="117"/>
       <c r="L529" s="30"/>
       <c r="M529" s="30"/>
       <c r="N529" s="30"/>
@@ -14466,7 +14504,7 @@
       <c r="H530" s="38"/>
       <c r="I530" s="38"/>
       <c r="J530" s="54"/>
-      <c r="K530" s="118"/>
+      <c r="K530" s="117"/>
       <c r="L530" s="30"/>
       <c r="M530" s="30"/>
       <c r="N530" s="30"/>
@@ -14486,7 +14524,7 @@
       <c r="H531" s="38"/>
       <c r="I531" s="38"/>
       <c r="J531" s="54"/>
-      <c r="K531" s="118"/>
+      <c r="K531" s="117"/>
       <c r="L531" s="30"/>
       <c r="M531" s="30"/>
       <c r="N531" s="30"/>
@@ -14506,7 +14544,7 @@
       <c r="H532" s="38"/>
       <c r="I532" s="38"/>
       <c r="J532" s="54"/>
-      <c r="K532" s="118"/>
+      <c r="K532" s="117"/>
       <c r="L532" s="30"/>
       <c r="M532" s="30"/>
       <c r="N532" s="30"/>
@@ -14526,7 +14564,7 @@
       <c r="H533" s="62"/>
       <c r="I533" s="62"/>
       <c r="J533" s="88"/>
-      <c r="K533" s="119"/>
+      <c r="K533" s="118"/>
       <c r="L533" s="76"/>
       <c r="M533" s="75"/>
       <c r="N533" s="75"/>
@@ -14866,7 +14904,7 @@
       <c r="H550" s="38"/>
       <c r="I550" s="38"/>
       <c r="J550" s="54"/>
-      <c r="K550" s="118"/>
+      <c r="K550" s="117"/>
       <c r="L550" s="30"/>
       <c r="M550" s="30"/>
       <c r="N550" s="30"/>
@@ -14886,7 +14924,7 @@
       <c r="H551" s="38"/>
       <c r="I551" s="38"/>
       <c r="J551" s="54"/>
-      <c r="K551" s="118"/>
+      <c r="K551" s="117"/>
       <c r="L551" s="30"/>
       <c r="M551" s="30"/>
       <c r="N551" s="30"/>
@@ -14906,7 +14944,7 @@
       <c r="H552" s="38"/>
       <c r="I552" s="38"/>
       <c r="J552" s="54"/>
-      <c r="K552" s="118"/>
+      <c r="K552" s="117"/>
       <c r="L552" s="30"/>
       <c r="M552" s="30"/>
       <c r="N552" s="30"/>
@@ -14926,7 +14964,7 @@
       <c r="H553" s="38"/>
       <c r="I553" s="38"/>
       <c r="J553" s="54"/>
-      <c r="K553" s="118"/>
+      <c r="K553" s="117"/>
       <c r="L553" s="30"/>
       <c r="M553" s="30"/>
       <c r="N553" s="30"/>
@@ -14946,7 +14984,7 @@
       <c r="H554" s="38"/>
       <c r="I554" s="38"/>
       <c r="J554" s="54"/>
-      <c r="K554" s="118"/>
+      <c r="K554" s="117"/>
       <c r="L554" s="30"/>
       <c r="M554" s="30"/>
       <c r="N554" s="30"/>
@@ -14966,7 +15004,7 @@
       <c r="H555" s="38"/>
       <c r="I555" s="38"/>
       <c r="J555" s="54"/>
-      <c r="K555" s="118"/>
+      <c r="K555" s="117"/>
       <c r="L555" s="30"/>
       <c r="M555" s="30"/>
       <c r="N555" s="30"/>
@@ -14986,7 +15024,7 @@
       <c r="H556" s="38"/>
       <c r="I556" s="38"/>
       <c r="J556" s="54"/>
-      <c r="K556" s="118"/>
+      <c r="K556" s="117"/>
       <c r="L556" s="30"/>
       <c r="M556" s="30"/>
       <c r="N556" s="30"/>
@@ -15006,7 +15044,7 @@
       <c r="H557" s="38"/>
       <c r="I557" s="38"/>
       <c r="J557" s="54"/>
-      <c r="K557" s="118"/>
+      <c r="K557" s="117"/>
       <c r="L557" s="30"/>
       <c r="M557" s="30"/>
       <c r="N557" s="30"/>
@@ -15026,7 +15064,7 @@
       <c r="H558" s="38"/>
       <c r="I558" s="38"/>
       <c r="J558" s="54"/>
-      <c r="K558" s="118"/>
+      <c r="K558" s="117"/>
       <c r="L558" s="30"/>
       <c r="M558" s="30"/>
       <c r="N558" s="30"/>
@@ -15046,7 +15084,7 @@
       <c r="H559" s="38"/>
       <c r="I559" s="38"/>
       <c r="J559" s="54"/>
-      <c r="K559" s="118"/>
+      <c r="K559" s="117"/>
       <c r="L559" s="30"/>
       <c r="M559" s="30"/>
       <c r="N559" s="30"/>
@@ -15066,7 +15104,7 @@
       <c r="H560" s="55"/>
       <c r="I560" s="55"/>
       <c r="J560" s="54"/>
-      <c r="K560" s="118"/>
+      <c r="K560" s="117"/>
       <c r="L560" s="30"/>
       <c r="M560" s="30"/>
       <c r="N560" s="30"/>
@@ -15086,7 +15124,7 @@
       <c r="H561" s="38"/>
       <c r="I561" s="38"/>
       <c r="J561" s="54"/>
-      <c r="K561" s="118"/>
+      <c r="K561" s="117"/>
       <c r="L561" s="30"/>
       <c r="M561" s="30"/>
       <c r="N561" s="30"/>
@@ -15106,7 +15144,7 @@
       <c r="H562" s="38"/>
       <c r="I562" s="38"/>
       <c r="J562" s="54"/>
-      <c r="K562" s="118"/>
+      <c r="K562" s="117"/>
       <c r="L562" s="30"/>
       <c r="M562" s="30"/>
       <c r="N562" s="30"/>
@@ -15126,7 +15164,7 @@
       <c r="H563" s="38"/>
       <c r="I563" s="38"/>
       <c r="J563" s="54"/>
-      <c r="K563" s="118"/>
+      <c r="K563" s="117"/>
       <c r="L563" s="30"/>
       <c r="M563" s="30"/>
       <c r="N563" s="30"/>
@@ -16126,7 +16164,7 @@
       <c r="H613" s="60"/>
       <c r="I613" s="60"/>
       <c r="J613" s="54"/>
-      <c r="K613" s="118"/>
+      <c r="K613" s="117"/>
       <c r="L613" s="30"/>
       <c r="M613" s="30"/>
       <c r="N613" s="30"/>
@@ -16146,7 +16184,7 @@
       <c r="H614" s="60"/>
       <c r="I614" s="60"/>
       <c r="J614" s="54"/>
-      <c r="K614" s="118"/>
+      <c r="K614" s="117"/>
       <c r="L614" s="30"/>
       <c r="M614" s="30"/>
       <c r="N614" s="30"/>
@@ -16166,7 +16204,7 @@
       <c r="H615" s="60"/>
       <c r="I615" s="60"/>
       <c r="J615" s="54"/>
-      <c r="K615" s="118"/>
+      <c r="K615" s="117"/>
       <c r="L615" s="30"/>
       <c r="M615" s="30"/>
       <c r="N615" s="30"/>
@@ -16186,7 +16224,7 @@
       <c r="H616" s="60"/>
       <c r="I616" s="60"/>
       <c r="J616" s="54"/>
-      <c r="K616" s="118"/>
+      <c r="K616" s="117"/>
       <c r="L616" s="30"/>
       <c r="M616" s="30"/>
       <c r="N616" s="30"/>
@@ -16206,7 +16244,7 @@
       <c r="H617" s="60"/>
       <c r="I617" s="60"/>
       <c r="J617" s="54"/>
-      <c r="K617" s="118"/>
+      <c r="K617" s="117"/>
       <c r="L617" s="30"/>
       <c r="M617" s="30"/>
       <c r="N617" s="30"/>
@@ -16226,7 +16264,7 @@
       <c r="H618" s="60"/>
       <c r="I618" s="60"/>
       <c r="J618" s="54"/>
-      <c r="K618" s="118"/>
+      <c r="K618" s="117"/>
       <c r="L618" s="30"/>
       <c r="M618" s="30"/>
       <c r="N618" s="30"/>
@@ -16586,7 +16624,7 @@
       <c r="H636" s="28"/>
       <c r="I636" s="28"/>
       <c r="J636" s="54"/>
-      <c r="K636" s="118"/>
+      <c r="K636" s="117"/>
       <c r="L636" s="28"/>
       <c r="M636" s="28"/>
       <c r="N636" s="28"/>
@@ -16606,7 +16644,7 @@
       <c r="H637" s="28"/>
       <c r="I637" s="28"/>
       <c r="J637" s="54"/>
-      <c r="K637" s="118"/>
+      <c r="K637" s="117"/>
       <c r="L637" s="28"/>
       <c r="M637" s="28"/>
       <c r="N637" s="28"/>
@@ -16626,7 +16664,7 @@
       <c r="H638" s="28"/>
       <c r="I638" s="28"/>
       <c r="J638" s="54"/>
-      <c r="K638" s="118"/>
+      <c r="K638" s="117"/>
       <c r="L638" s="28"/>
       <c r="M638" s="28"/>
       <c r="N638" s="28"/>
@@ -16646,7 +16684,7 @@
       <c r="H639" s="28"/>
       <c r="I639" s="28"/>
       <c r="J639" s="54"/>
-      <c r="K639" s="118"/>
+      <c r="K639" s="117"/>
       <c r="L639" s="28"/>
       <c r="M639" s="28"/>
       <c r="N639" s="28"/>
@@ -16666,7 +16704,7 @@
       <c r="H640" s="28"/>
       <c r="I640" s="28"/>
       <c r="J640" s="54"/>
-      <c r="K640" s="118"/>
+      <c r="K640" s="117"/>
       <c r="L640" s="28"/>
       <c r="M640" s="28"/>
       <c r="N640" s="28"/>
@@ -16966,7 +17004,7 @@
       <c r="H655" s="27"/>
       <c r="I655" s="27"/>
       <c r="J655" s="54"/>
-      <c r="K655" s="118"/>
+      <c r="K655" s="117"/>
       <c r="L655" s="28"/>
       <c r="M655" s="28"/>
       <c r="N655" s="28"/>
@@ -17086,7 +17124,7 @@
       <c r="H661" s="27"/>
       <c r="I661" s="27"/>
       <c r="J661" s="54"/>
-      <c r="K661" s="118"/>
+      <c r="K661" s="117"/>
       <c r="L661" s="28"/>
       <c r="M661" s="28"/>
       <c r="N661" s="28"/>
@@ -17126,7 +17164,7 @@
       <c r="H663" s="27"/>
       <c r="I663" s="27"/>
       <c r="J663" s="54"/>
-      <c r="K663" s="118"/>
+      <c r="K663" s="117"/>
       <c r="L663" s="28"/>
       <c r="M663" s="28"/>
       <c r="N663" s="28"/>
@@ -17186,7 +17224,7 @@
       <c r="H666" s="27"/>
       <c r="I666" s="27"/>
       <c r="J666" s="54"/>
-      <c r="K666" s="118"/>
+      <c r="K666" s="117"/>
       <c r="L666" s="28"/>
       <c r="M666" s="28"/>
       <c r="N666" s="28"/>
@@ -17486,7 +17524,7 @@
       <c r="H681" s="27"/>
       <c r="I681" s="27"/>
       <c r="J681" s="54"/>
-      <c r="K681" s="118"/>
+      <c r="K681" s="117"/>
       <c r="L681" s="28"/>
       <c r="M681" s="28"/>
       <c r="N681" s="28"/>
@@ -17546,7 +17584,7 @@
       <c r="H684" s="27"/>
       <c r="I684" s="27"/>
       <c r="J684" s="54"/>
-      <c r="K684" s="118"/>
+      <c r="K684" s="117"/>
       <c r="L684" s="28"/>
       <c r="M684" s="28"/>
       <c r="N684" s="28"/>
@@ -17646,7 +17684,7 @@
       <c r="H689" s="27"/>
       <c r="I689" s="27"/>
       <c r="J689" s="87"/>
-      <c r="K689" s="120"/>
+      <c r="K689" s="119"/>
       <c r="L689" s="28"/>
       <c r="M689" s="28"/>
       <c r="N689" s="28"/>
@@ -17746,7 +17784,7 @@
       <c r="H694" s="27"/>
       <c r="I694" s="27"/>
       <c r="J694" s="54"/>
-      <c r="K694" s="118"/>
+      <c r="K694" s="117"/>
       <c r="L694" s="28"/>
       <c r="M694" s="28"/>
       <c r="N694" s="28"/>
@@ -17786,7 +17824,7 @@
       <c r="H696" s="27"/>
       <c r="I696" s="27"/>
       <c r="J696" s="54"/>
-      <c r="K696" s="118"/>
+      <c r="K696" s="117"/>
       <c r="L696" s="28"/>
       <c r="M696" s="28"/>
       <c r="N696" s="28"/>
@@ -18146,7 +18184,7 @@
       <c r="H714" s="38"/>
       <c r="I714" s="38"/>
       <c r="J714" s="54"/>
-      <c r="K714" s="118"/>
+      <c r="K714" s="117"/>
       <c r="L714" s="30"/>
       <c r="M714" s="30"/>
       <c r="N714" s="30"/>
@@ -18166,7 +18204,7 @@
       <c r="H715" s="38"/>
       <c r="I715" s="38"/>
       <c r="J715" s="54"/>
-      <c r="K715" s="118"/>
+      <c r="K715" s="117"/>
       <c r="L715" s="30"/>
       <c r="M715" s="30"/>
       <c r="N715" s="30"/>
@@ -18186,7 +18224,7 @@
       <c r="H716" s="38"/>
       <c r="I716" s="38"/>
       <c r="J716" s="54"/>
-      <c r="K716" s="118"/>
+      <c r="K716" s="117"/>
       <c r="L716" s="30"/>
       <c r="M716" s="30"/>
       <c r="N716" s="30"/>
@@ -18206,7 +18244,7 @@
       <c r="H717" s="38"/>
       <c r="I717" s="38"/>
       <c r="J717" s="54"/>
-      <c r="K717" s="118"/>
+      <c r="K717" s="117"/>
       <c r="L717" s="30"/>
       <c r="M717" s="30"/>
       <c r="N717" s="30"/>
@@ -18226,7 +18264,7 @@
       <c r="H718" s="38"/>
       <c r="I718" s="38"/>
       <c r="J718" s="54"/>
-      <c r="K718" s="118"/>
+      <c r="K718" s="117"/>
       <c r="L718" s="30"/>
       <c r="M718" s="30"/>
       <c r="N718" s="30"/>
@@ -18246,7 +18284,7 @@
       <c r="H719" s="38"/>
       <c r="I719" s="38"/>
       <c r="J719" s="54"/>
-      <c r="K719" s="118"/>
+      <c r="K719" s="117"/>
       <c r="L719" s="30"/>
       <c r="M719" s="30"/>
       <c r="N719" s="30"/>
@@ -18266,7 +18304,7 @@
       <c r="H720" s="38"/>
       <c r="I720" s="38"/>
       <c r="J720" s="54"/>
-      <c r="K720" s="118"/>
+      <c r="K720" s="117"/>
       <c r="L720" s="30"/>
       <c r="M720" s="30"/>
       <c r="N720" s="30"/>
@@ -18286,7 +18324,7 @@
       <c r="H721" s="38"/>
       <c r="I721" s="38"/>
       <c r="J721" s="54"/>
-      <c r="K721" s="118"/>
+      <c r="K721" s="117"/>
       <c r="L721" s="30"/>
       <c r="M721" s="30"/>
       <c r="N721" s="30"/>
@@ -18306,7 +18344,7 @@
       <c r="H722" s="38"/>
       <c r="I722" s="38"/>
       <c r="J722" s="87"/>
-      <c r="K722" s="120"/>
+      <c r="K722" s="119"/>
       <c r="L722" s="30"/>
       <c r="M722" s="30"/>
       <c r="N722" s="30"/>
@@ -19186,7 +19224,7 @@
       <c r="H766" s="38"/>
       <c r="I766" s="38"/>
       <c r="J766" s="54"/>
-      <c r="K766" s="118"/>
+      <c r="K766" s="117"/>
       <c r="L766" s="30"/>
       <c r="M766" s="30"/>
       <c r="N766" s="30"/>
@@ -19206,7 +19244,7 @@
       <c r="H767" s="38"/>
       <c r="I767" s="38"/>
       <c r="J767" s="54"/>
-      <c r="K767" s="118"/>
+      <c r="K767" s="117"/>
       <c r="L767" s="30"/>
       <c r="M767" s="30"/>
       <c r="N767" s="30"/>
@@ -19226,7 +19264,7 @@
       <c r="H768" s="38"/>
       <c r="I768" s="38"/>
       <c r="J768" s="54"/>
-      <c r="K768" s="118"/>
+      <c r="K768" s="117"/>
       <c r="L768" s="30"/>
       <c r="M768" s="30"/>
       <c r="N768" s="30"/>
@@ -19246,7 +19284,7 @@
       <c r="H769" s="38"/>
       <c r="I769" s="38"/>
       <c r="J769" s="54"/>
-      <c r="K769" s="118"/>
+      <c r="K769" s="117"/>
       <c r="L769" s="30"/>
       <c r="M769" s="30"/>
       <c r="N769" s="30"/>
@@ -19266,7 +19304,7 @@
       <c r="H770" s="24"/>
       <c r="I770" s="24"/>
       <c r="J770" s="54"/>
-      <c r="K770" s="118"/>
+      <c r="K770" s="117"/>
       <c r="L770" s="30"/>
       <c r="M770" s="30"/>
       <c r="N770" s="30"/>
@@ -19286,7 +19324,7 @@
       <c r="H771" s="24"/>
       <c r="I771" s="24"/>
       <c r="J771" s="54"/>
-      <c r="K771" s="118"/>
+      <c r="K771" s="117"/>
       <c r="L771" s="30"/>
       <c r="M771" s="30"/>
       <c r="N771" s="30"/>
@@ -19306,7 +19344,7 @@
       <c r="H772" s="38"/>
       <c r="I772" s="38"/>
       <c r="J772" s="54"/>
-      <c r="K772" s="118"/>
+      <c r="K772" s="117"/>
       <c r="L772" s="30"/>
       <c r="M772" s="30"/>
       <c r="N772" s="30"/>
@@ -19706,7 +19744,7 @@
       <c r="H792" s="27"/>
       <c r="I792" s="27"/>
       <c r="J792" s="54"/>
-      <c r="K792" s="118"/>
+      <c r="K792" s="117"/>
       <c r="L792" s="28"/>
       <c r="M792" s="28"/>
       <c r="N792" s="28"/>
@@ -19866,7 +19904,7 @@
       <c r="H800" s="27"/>
       <c r="I800" s="27"/>
       <c r="J800" s="54"/>
-      <c r="K800" s="118"/>
+      <c r="K800" s="117"/>
       <c r="L800" s="28"/>
       <c r="M800" s="28"/>
       <c r="N800" s="28"/>
@@ -20086,7 +20124,7 @@
       <c r="H811" s="27"/>
       <c r="I811" s="27"/>
       <c r="J811" s="54"/>
-      <c r="K811" s="118"/>
+      <c r="K811" s="117"/>
       <c r="L811" s="28"/>
       <c r="M811" s="28"/>
       <c r="N811" s="28"/>
@@ -20106,7 +20144,7 @@
       <c r="H812" s="27"/>
       <c r="I812" s="27"/>
       <c r="J812" s="54"/>
-      <c r="K812" s="118"/>
+      <c r="K812" s="117"/>
       <c r="L812" s="28"/>
       <c r="M812" s="28"/>
       <c r="N812" s="28"/>
@@ -20126,7 +20164,7 @@
       <c r="H813" s="27"/>
       <c r="I813" s="27"/>
       <c r="J813" s="54"/>
-      <c r="K813" s="118"/>
+      <c r="K813" s="117"/>
       <c r="L813" s="28"/>
       <c r="M813" s="28"/>
       <c r="N813" s="28"/>
@@ -20146,7 +20184,7 @@
       <c r="H814" s="27"/>
       <c r="I814" s="27"/>
       <c r="J814" s="54"/>
-      <c r="K814" s="118"/>
+      <c r="K814" s="117"/>
       <c r="L814" s="28"/>
       <c r="M814" s="28"/>
       <c r="N814" s="28"/>
@@ -20166,7 +20204,7 @@
       <c r="H815" s="27"/>
       <c r="I815" s="27"/>
       <c r="J815" s="54"/>
-      <c r="K815" s="118"/>
+      <c r="K815" s="117"/>
       <c r="L815" s="28"/>
       <c r="M815" s="28"/>
       <c r="N815" s="28"/>
@@ -20186,7 +20224,7 @@
       <c r="H816" s="27"/>
       <c r="I816" s="27"/>
       <c r="J816" s="54"/>
-      <c r="K816" s="118"/>
+      <c r="K816" s="117"/>
       <c r="L816" s="28"/>
       <c r="M816" s="28"/>
       <c r="N816" s="28"/>
@@ -20206,7 +20244,7 @@
       <c r="H817" s="27"/>
       <c r="I817" s="27"/>
       <c r="J817" s="54"/>
-      <c r="K817" s="118"/>
+      <c r="K817" s="117"/>
       <c r="L817" s="28"/>
       <c r="M817" s="28"/>
       <c r="N817" s="28"/>
@@ -20226,7 +20264,7 @@
       <c r="H818" s="27"/>
       <c r="I818" s="27"/>
       <c r="J818" s="54"/>
-      <c r="K818" s="118"/>
+      <c r="K818" s="117"/>
       <c r="L818" s="28"/>
       <c r="M818" s="28"/>
       <c r="N818" s="28"/>
@@ -20246,7 +20284,7 @@
       <c r="H819" s="27"/>
       <c r="I819" s="27"/>
       <c r="J819" s="54"/>
-      <c r="K819" s="118"/>
+      <c r="K819" s="117"/>
       <c r="L819" s="28"/>
       <c r="M819" s="28"/>
       <c r="N819" s="28"/>
@@ -20386,7 +20424,7 @@
       <c r="H826" s="38"/>
       <c r="I826" s="38"/>
       <c r="J826" s="54"/>
-      <c r="K826" s="118"/>
+      <c r="K826" s="117"/>
       <c r="L826" s="30"/>
       <c r="M826" s="30"/>
       <c r="N826" s="30"/>
@@ -20900,6 +20938,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:R850">
+    <filterColumn colId="1">
+      <filters blank="1">
+        <filter val="5.Profil"/>
+      </filters>
+    </filterColumn>
     <sortState ref="A2:Y864">
       <sortCondition ref="B1:B864"/>
     </sortState>
@@ -20938,21 +20981,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003DF93D1C80BCE4439E37126069156F2D" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ac6bdae7674316788986ea2d0cdff43d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -21001,10 +21029,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56277F14-5102-450B-9F74-CC1199F0A7EB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA27FEB7-001F-49B4-9822-FC9222977738}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -21024,16 +21074,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA27FEB7-001F-49B4-9822-FC9222977738}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56277F14-5102-450B-9F74-CC1199F0A7EB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>